<commit_message>
fixed bugs in navantaj.py
</commit_message>
<xml_diff>
--- a/Копия Овсов_таблиця складу рентабельності групи.xlsx
+++ b/Копия Овсов_таблиця складу рентабельності групи.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Учеба\8_семестр\диплом\term_paper_3d_grade\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB71EAB7-E423-42A9-A0CD-8CF95A60A023}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Бакалавр" sheetId="1" r:id="rId1"/>
+    <sheet name="Бакалавр" sheetId="4" r:id="rId1"/>
     <sheet name="звед дані рентаб(контракт)" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -72,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,15 +138,15 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -214,7 +208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,26 +241,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,23 +276,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -491,11 +451,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +542,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" ref="C8:C17" si="0">CEILING(($D$4-B8*$D$7)/$E$7,1)</f>
+        <f>CEILING(($D$4-B8*$D$7)/$E$7,1)</f>
         <v>15</v>
       </c>
     </row>
@@ -591,7 +551,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" si="0"/>
+        <f>CEILING(($D$4-B9*$D$7)/$E$7,1)</f>
         <v>13</v>
       </c>
     </row>
@@ -600,7 +560,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" si="0"/>
+        <f>CEILING(($D$4-B10*$D$7)/$E$7,1)</f>
         <v>12</v>
       </c>
     </row>
@@ -609,7 +569,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" si="0"/>
+        <f>CEILING(($D$4-B11*$D$7)/$E$7,1)</f>
         <v>10</v>
       </c>
     </row>
@@ -618,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="4">
-        <f t="shared" si="0"/>
+        <f>CEILING(($D$4-B12*$D$7)/$E$7,1)</f>
         <v>8</v>
       </c>
     </row>
@@ -627,7 +587,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="4">
-        <f t="shared" si="0"/>
+        <f>CEILING(($D$4-B13*$D$7)/$E$7,1)</f>
         <v>7</v>
       </c>
     </row>
@@ -636,7 +596,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" si="0"/>
+        <f>CEILING(($D$4-B14*$D$7)/$E$7,1)</f>
         <v>5</v>
       </c>
     </row>
@@ -645,7 +605,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="4">
-        <f t="shared" si="0"/>
+        <f>CEILING(($D$4-B15*$D$7)/$E$7,1)</f>
         <v>3</v>
       </c>
     </row>
@@ -654,7 +614,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="4">
-        <f t="shared" si="0"/>
+        <f>CEILING(($D$4-B16*$D$7)/$E$7,1)</f>
         <v>2</v>
       </c>
     </row>
@@ -666,7 +626,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" si="0"/>
+        <f>CEILING(($D$4-B17*$D$7)/$E$7,1)</f>
         <v>0</v>
       </c>
     </row>
@@ -677,10 +637,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J16"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -692,14 +652,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
@@ -712,19 +672,19 @@
       <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>10</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>12</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>14</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <v>16</v>
       </c>
     </row>
@@ -745,19 +705,19 @@
         <f>D5*C5</f>
         <v>530684</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <f>$E5/$G$4</f>
         <v>53068.4</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <f>$E5/$H$4</f>
         <v>44223.666666666664</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <f>$E5/$I$4</f>
         <v>37906</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="7">
         <f>$E5/$J$4</f>
         <v>33167.75</v>
       </c>
@@ -776,19 +736,19 @@
         <f>D6*C6</f>
         <v>604140</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <f t="shared" ref="G6:G16" si="0">$E6/$G$4</f>
         <v>60414</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <f t="shared" ref="H6:H16" si="1">$E6/$H$4</f>
         <v>50345</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <f t="shared" ref="I6:I16" si="2">$E6/$I$4</f>
         <v>43152.857142857145</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="7">
         <f t="shared" ref="J6:J16" si="3">$E6/$J$4</f>
         <v>37758.75</v>
       </c>
@@ -807,19 +767,19 @@
         <f t="shared" ref="E7:E16" si="4">D7*C7</f>
         <v>681798</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <f t="shared" si="0"/>
         <v>68179.8</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <f t="shared" si="1"/>
         <v>56816.5</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <f t="shared" si="2"/>
         <v>48699.857142857145</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="7">
         <f t="shared" si="3"/>
         <v>42612.375</v>
       </c>
@@ -838,19 +798,19 @@
         <f t="shared" si="4"/>
         <v>763658</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <f t="shared" si="0"/>
         <v>76365.8</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <f t="shared" si="1"/>
         <v>63638.166666666664</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <f t="shared" si="2"/>
         <v>54547</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="7">
         <f t="shared" si="3"/>
         <v>47728.625</v>
       </c>
@@ -869,19 +829,19 @@
         <f t="shared" si="4"/>
         <v>849720</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <f t="shared" si="0"/>
         <v>84972</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <f t="shared" si="1"/>
         <v>70810</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <f t="shared" si="2"/>
         <v>60694.285714285717</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="7">
         <f t="shared" si="3"/>
         <v>53107.5</v>
       </c>
@@ -900,19 +860,19 @@
         <f t="shared" si="4"/>
         <v>939984</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
         <v>93998.399999999994</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <f t="shared" si="1"/>
         <v>78332</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <f t="shared" si="2"/>
         <v>67141.71428571429</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="7">
         <f t="shared" si="3"/>
         <v>58749</v>
       </c>
@@ -931,19 +891,19 @@
         <f t="shared" si="4"/>
         <v>1034450</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <f t="shared" si="0"/>
         <v>103445</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <f t="shared" si="1"/>
         <v>86204.166666666672</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <f t="shared" si="2"/>
         <v>73889.28571428571</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="7">
         <f t="shared" si="3"/>
         <v>64653.125</v>
       </c>
@@ -962,19 +922,19 @@
         <f t="shared" si="4"/>
         <v>1133118</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <f t="shared" si="0"/>
         <v>113311.8</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <f t="shared" si="1"/>
         <v>94426.5</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <f t="shared" si="2"/>
         <v>80937</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="7">
         <f t="shared" si="3"/>
         <v>70819.875</v>
       </c>
@@ -993,19 +953,19 @@
         <f t="shared" si="4"/>
         <v>1235988</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <f t="shared" si="0"/>
         <v>123598.8</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <f t="shared" si="1"/>
         <v>102999</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <f t="shared" si="2"/>
         <v>88284.857142857145</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="7">
         <f t="shared" si="3"/>
         <v>77249.25</v>
       </c>
@@ -1024,19 +984,19 @@
         <f t="shared" si="4"/>
         <v>1343060</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <f t="shared" si="0"/>
         <v>134306</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <f t="shared" si="1"/>
         <v>111921.66666666667</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <f t="shared" si="2"/>
         <v>95932.857142857145</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="7">
         <f t="shared" si="3"/>
         <v>83941.25</v>
       </c>
@@ -1055,19 +1015,19 @@
         <f t="shared" si="4"/>
         <v>1454334</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <f t="shared" si="0"/>
         <v>145433.4</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="7">
         <f t="shared" si="1"/>
         <v>121194.5</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <f t="shared" si="2"/>
         <v>103881</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="7">
         <f t="shared" si="3"/>
         <v>90895.875</v>
       </c>
@@ -1086,19 +1046,19 @@
         <f t="shared" si="4"/>
         <v>1569810</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <f t="shared" si="0"/>
         <v>156981</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <f t="shared" si="1"/>
         <v>130817.5</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="7">
         <f t="shared" si="2"/>
         <v>112129.28571428571</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="7">
         <f t="shared" si="3"/>
         <v>98113.125</v>
       </c>
@@ -1112,7 +1072,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>